<commit_message>
Update 28-06-2016 for phuhl
</commit_message>
<xml_diff>
--- a/phuhl/Data.xlsx
+++ b/phuhl/Data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="HistoryChange" sheetId="2" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="99">
   <si>
     <t>Ngày</t>
   </si>
@@ -33,13 +33,300 @@
   </si>
   <si>
     <t>Link - trang web</t>
+  </si>
+  <si>
+    <t>CÔNG TY CỔ PHẦN PHẦN MỀM SS4U</t>
+  </si>
+  <si>
+    <t>http://ss4u.vn/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Công ty Cổ Phần Dịch Vụ Đông Tiến (DTSC) </t>
+  </si>
+  <si>
+    <t>http://www.dtsc.vn/</t>
+  </si>
+  <si>
+    <t>Địa chỉ</t>
+  </si>
+  <si>
+    <t>Lầu 4, 418 Trần Phú, Phường 7, Quận 5, TP.HCM .</t>
+  </si>
+  <si>
+    <t>Lầu 5A, Tòa nhà Green Star, 70 Phạm Ngọc Thạch, Quận 3, TP HCM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Công ty Squarebit Studio </t>
+  </si>
+  <si>
+    <t>Công ty Precio</t>
+  </si>
+  <si>
+    <t>CÔNG TY TNHH VINAHOST</t>
+  </si>
+  <si>
+    <t>http://vinahost.vn</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 351/31 Nơ Trang Long, P.13, Q. Bình Thạnh, TP. HCM</t>
+  </si>
+  <si>
+    <t>http://squarebit.studio/</t>
+  </si>
+  <si>
+    <t>93 (số cũ 1179), Hiệp Nhất, Phường 14, Quận Tân Bình, TP.HCM</t>
+  </si>
+  <si>
+    <t>http://www.preciofishbone.se/en/</t>
+  </si>
+  <si>
+    <t>Công ty FPT Software</t>
+  </si>
+  <si>
+    <t>Công ty Faceseo</t>
+  </si>
+  <si>
+    <t>http://faceseo.vn/</t>
+  </si>
+  <si>
+    <t>36 đường A4, P 12, Q Tân Bình, Hồ Chí Minh</t>
+  </si>
+  <si>
+    <t>Lô T2, đường D1, khu Công viên công nghệ cao Sài Gòn, quận 9, Hồ Chí Minh</t>
+  </si>
+  <si>
+    <t>Trụ sở chính : nước ngoài</t>
+  </si>
+  <si>
+    <t>STT</t>
+  </si>
+  <si>
+    <t>Công ty Emotive Software Co., Ltd</t>
+  </si>
+  <si>
+    <t>http://emotive.de/</t>
+  </si>
+  <si>
+    <t>235/44 đường Trục, P.13, Q.Bình Thạnh, Tp.HCM.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Công ty Orient Software </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Công ty SystemEXE </t>
+  </si>
+  <si>
+    <t>http://www.orientsoftware.net</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5th floor, Suite 5.8, e.town 1 building, 364 Cong Hoa Str, 
+Ward 13, Tan Binh Dist, Ho Chi Minh </t>
+  </si>
+  <si>
+    <t>http://www.system-exe.com.vn</t>
+  </si>
+  <si>
+    <t>Lầu 4, Etown 1, 364 Cộng Hòa, P.13, Q.Tân Bình</t>
+  </si>
+  <si>
+    <t>Công ty TNHH CSCOM</t>
+  </si>
+  <si>
+    <t>www.cscom.vn</t>
+  </si>
+  <si>
+    <t>357 Lê Hồng Phong, Phường 2, Quận 10, Tp. Hồ Chí Minh</t>
+  </si>
+  <si>
+    <t>Axon Active Vietnam</t>
+  </si>
+  <si>
+    <t>http://www.axonactive.vn/</t>
+  </si>
+  <si>
+    <t>https://career.fpt-software.com/vn/
+http://fpt-software.com/</t>
+  </si>
+  <si>
+    <t>Hai Au Building 10th Floor, 39B Truong Son Str., Ward 4,
+ Tan Binh Dist., Ho Chi Minh City, Vietnam</t>
+  </si>
+  <si>
+    <t>Công Ty Tnhh Sparx Việt Nam</t>
+  </si>
+  <si>
+    <t>http://www.sgs.vn/</t>
+  </si>
+  <si>
+    <t>141 Lý Chính Thắng, 7, 3, Hồ Chí Minh, Vietnam</t>
+  </si>
+  <si>
+    <t>CÔNG TY TNHH BRIGHTS VIỆT NAM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">135/37/1 Nguyễn Hữu Cảnh, phường 22, quận Bình Thạnh,Thành phố Hồ </t>
+  </si>
+  <si>
+    <t>http://brights.vn/vi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tòa nhà WASECO, 10 Phổ Quang, Quận Tân Bình, Thành phố Hồ Chí </t>
+  </si>
+  <si>
+    <t>http://www.fujinet.net/</t>
+  </si>
+  <si>
+    <t>Vinagame</t>
+  </si>
+  <si>
+    <t>182 Lê Đại Hành, Phường 15, Quận 11, Thành phố Hồ Chí Minh</t>
+  </si>
+  <si>
+    <t>http://vng.com.vn/</t>
+  </si>
+  <si>
+    <t>Công ty Gameloft Việt Nam</t>
+  </si>
+  <si>
+    <t>Công ty Fujinet Systems JSC</t>
+  </si>
+  <si>
+    <t>CSC Việt Nam</t>
+  </si>
+  <si>
+    <t>366 Nguyen Trai, District 5, HCMC | Branch Office: Etown 3 - 364
+ Cong Hoa, Tan Binh, HCMC</t>
+  </si>
+  <si>
+    <t>http://www.csc.com/</t>
+  </si>
+  <si>
+    <t>KMS VIET NAM CO., LTD</t>
+  </si>
+  <si>
+    <t>123 Cong Hoa Street, Tan Binh District, HCMC / 191B Hoang Van Thu Street,
+ Phu Nhuan District, HCMC / 17 Ho Van Hue Street, Phu Nhuan District, HCMC</t>
+  </si>
+  <si>
+    <t>http://www.kms-technology.com/</t>
+  </si>
+  <si>
+    <t>http://www.gameloft.vn</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 18A, Cộng Hòa, Phường 12, Hồ Chí Minh</t>
+  </si>
+  <si>
+    <t>http://www.isb-vietnam.com.vn</t>
+  </si>
+  <si>
+    <t>ISB việt nam</t>
+  </si>
+  <si>
+    <t>Unit 3.1, 3rd Floor, E-town 2 Building
+364 Cong Hoa, Tan Binh Dist, HCM City, Vietnam</t>
+  </si>
+  <si>
+    <t>TMA (Tường Minh)</t>
+  </si>
+  <si>
+    <t>http://www.tmasolutions.com/</t>
+  </si>
+  <si>
+    <t>TMA Tower, Quang Trung Software City, District 12</t>
+  </si>
+  <si>
+    <t>Công ty CityNow</t>
+  </si>
+  <si>
+    <t>citynowinc@gmail.com</t>
+  </si>
+  <si>
+    <t>298 Đường 3/2, Phường 12, Quận 10, TP Hồ Chí Minh</t>
+  </si>
+  <si>
+    <t>https://naustud.io/</t>
+  </si>
+  <si>
+    <t>Công ty Works Applications - Nhật Bản</t>
+  </si>
+  <si>
+    <t>http://www.worksap.com/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Công ty TNHH Sáng tạo Nâu | Nau Creative Co. Ltd. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">187A/2 Dien Bien Phu, Da Kao Ward, District 1, Ho Chi Minh City, Viet Nam. </t>
+  </si>
+  <si>
+    <t>Công ty Pinride</t>
+  </si>
+  <si>
+    <t>54/09 Dao Duy Anh, Phu Nhuan, Ho Chi Minh City</t>
+  </si>
+  <si>
+    <t>hackers@pinride.me</t>
+  </si>
+  <si>
+    <t>Công ty TNHH Thiết kế Renesas Việt Nam tuyển</t>
+  </si>
+  <si>
+    <t>http://vietnam.renesas.com/</t>
+  </si>
+  <si>
+    <t>http://www.topcareer.jp/inter/job/detail/001552/
+https://www.facebook.com/topcareervietnam/</t>
+  </si>
+  <si>
+    <t>Công ty Evolution Solutions</t>
+  </si>
+  <si>
+    <t>http://www.evolus.vn</t>
+  </si>
+  <si>
+    <t>Tầng 2, Toà nhà PHL, 109 Cộng Hòa, Phường 12, Quận Tân Bình, Thành phố Hồ Chí Minh, Việt Nam.</t>
+  </si>
+  <si>
+    <t>Công ty Ryomo Vietnam Solutions</t>
+  </si>
+  <si>
+    <t>http://rvsc.ryomo-gr.com</t>
+  </si>
+  <si>
+    <t>Lot W.29-30-31a, Tan Thuan Road, Tan Thuan Export 
+Processing Zone, District 7, Ho Chi Minh City, Vietnam</t>
+  </si>
+  <si>
+    <t>Phòng 605-08, Lầu 6, Tòa nhà Saigon Riverside Office Center, 2A-4A đường Tôn Đức Thắng, quận 1, thành phố Hồ Chí Minh, Việt Nam.</t>
+  </si>
+  <si>
+    <t>Công ty Lampart</t>
+  </si>
+  <si>
+    <t>http://lampart-vn.com/en/</t>
+  </si>
+  <si>
+    <t>23 Nguyen Phi Khanh Str, Tan Dinh Ward, District 1, HCMC, VietNam</t>
+  </si>
+  <si>
+    <t>28-06-2016</t>
+  </si>
+  <si>
+    <t>Add stt: 1-&gt;29</t>
+  </si>
+  <si>
+    <t>Tác giả</t>
+  </si>
+  <si>
+    <t>Phú Lê</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -51,6 +338,14 @@
       <b/>
       <sz val="11"/>
       <color theme="3" tint="0.79998168889431442"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -79,10 +374,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -90,8 +386,24 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -394,32 +706,50 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:C4"/>
+  <dimension ref="B3:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="17.140625" customWidth="1"/>
     <col min="3" max="3" width="44" customWidth="1"/>
+    <col min="4" max="4" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D3" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>3</v>
+      </c>
+      <c r="D4" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B5" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D5" t="s">
+        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -430,27 +760,474 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:C2"/>
+  <dimension ref="A2:D31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="20.28515625" customWidth="1"/>
-    <col min="3" max="3" width="50.85546875" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="64.140625" customWidth="1"/>
+    <col min="3" max="3" width="37.85546875" customWidth="1"/>
+    <col min="4" max="4" width="69.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>27</v>
+      </c>
       <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>5</v>
       </c>
+      <c r="D2" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" s="3" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>6</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>7</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>8</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" s="3" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>9</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>10</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>11</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" s="3" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>12</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>13</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>14</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>15</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>16</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>17</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" s="3" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>18</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" s="3" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>19</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" s="3" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>20</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>21</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>22</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>23</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" s="3" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>24</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <v>25</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="D27" s="7" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
+        <v>26</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="D28" s="7" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
+        <v>27</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="D29" s="7" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" s="3" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
+        <v>28</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="D30" s="7" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
+        <v>29</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>94</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C3" r:id="rId1"/>
+    <hyperlink ref="C4" r:id="rId2"/>
+    <hyperlink ref="C7" r:id="rId3"/>
+    <hyperlink ref="C5" r:id="rId4"/>
+    <hyperlink ref="C6" r:id="rId5"/>
+    <hyperlink ref="C8" r:id="rId6" display="https://career.fpt-software.com/vn/"/>
+    <hyperlink ref="C9" r:id="rId7"/>
+    <hyperlink ref="C10" r:id="rId8"/>
+    <hyperlink ref="C11" r:id="rId9"/>
+    <hyperlink ref="C12" r:id="rId10"/>
+    <hyperlink ref="C13" r:id="rId11"/>
+    <hyperlink ref="C14" r:id="rId12"/>
+    <hyperlink ref="C15" r:id="rId13"/>
+    <hyperlink ref="C16" r:id="rId14"/>
+    <hyperlink ref="C17" r:id="rId15"/>
+    <hyperlink ref="C18" r:id="rId16"/>
+    <hyperlink ref="C20" r:id="rId17"/>
+    <hyperlink ref="C21" r:id="rId18"/>
+    <hyperlink ref="C19" r:id="rId19"/>
+    <hyperlink ref="C22" r:id="rId20"/>
+    <hyperlink ref="C23" r:id="rId21"/>
+    <hyperlink ref="C24" r:id="rId22"/>
+    <hyperlink ref="C25" r:id="rId23"/>
+    <hyperlink ref="C26" r:id="rId24"/>
+    <hyperlink ref="C27" r:id="rId25"/>
+    <hyperlink ref="C28" r:id="rId26"/>
+    <hyperlink ref="D26" r:id="rId27" display="http://www.topcareer.jp/inter/job/detail/001552/"/>
+    <hyperlink ref="C29" r:id="rId28"/>
+    <hyperlink ref="C30" r:id="rId29"/>
+    <hyperlink ref="C31" r:id="rId30"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId31"/>
 </worksheet>
 </file>
</xml_diff>